<commit_message>
Updating stable version of code and initializing documentation
</commit_message>
<xml_diff>
--- a/01_Planning/Radar Odometry Planning.xlsx
+++ b/01_Planning/Radar Odometry Planning.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="366" documentId="8_{52EDD424-5212-40DD-83C2-A60CD23DB59C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F7E25A1-93A1-48FA-A69C-623362F9EC4E}"/>
+  <xr:revisionPtr revIDLastSave="367" documentId="8_{52EDD424-5212-40DD-83C2-A60CD23DB59C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B68C8810-2E86-42FD-B0BA-8CE1D79D4C75}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -686,6 +686,36 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="8" borderId="0" xfId="6" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="9" borderId="0" xfId="6" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -718,36 +748,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="8" borderId="0" xfId="6" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="9" borderId="0" xfId="6" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -925,10 +925,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1164,8 +1160,8 @@
   </sheetPr>
   <dimension ref="B1:BO49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1199,69 +1195,69 @@
         <v>17</v>
       </c>
       <c r="H2" s="14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J2" s="15"/>
-      <c r="K2" s="30" t="s">
+      <c r="K2" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="32"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="42"/>
       <c r="P2" s="16"/>
-      <c r="Q2" s="30" t="s">
+      <c r="Q2" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="32"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="42"/>
       <c r="U2" s="17"/>
-      <c r="V2" s="24" t="s">
+      <c r="V2" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="W2" s="25"/>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="34"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="44"/>
       <c r="Z2" s="18"/>
-      <c r="AA2" s="24" t="s">
+      <c r="AA2" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="AB2" s="25"/>
-      <c r="AC2" s="25"/>
-      <c r="AD2" s="25"/>
-      <c r="AE2" s="25"/>
-      <c r="AF2" s="25"/>
-      <c r="AG2" s="34"/>
+      <c r="AB2" s="35"/>
+      <c r="AC2" s="35"/>
+      <c r="AD2" s="35"/>
+      <c r="AE2" s="35"/>
+      <c r="AF2" s="35"/>
+      <c r="AG2" s="44"/>
       <c r="AH2" s="19"/>
-      <c r="AI2" s="24" t="s">
+      <c r="AI2" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="AJ2" s="25"/>
-      <c r="AK2" s="25"/>
-      <c r="AL2" s="25"/>
-      <c r="AM2" s="25"/>
-      <c r="AN2" s="25"/>
-      <c r="AO2" s="25"/>
-      <c r="AP2" s="25"/>
+      <c r="AJ2" s="35"/>
+      <c r="AK2" s="35"/>
+      <c r="AL2" s="35"/>
+      <c r="AM2" s="35"/>
+      <c r="AN2" s="35"/>
+      <c r="AO2" s="35"/>
+      <c r="AP2" s="35"/>
     </row>
     <row r="3" spans="2:67" s="11" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="39" t="s">
         <v>22</v>
       </c>
       <c r="H3" s="20" t="s">
@@ -1288,12 +1284,12 @@
       <c r="AA3" s="10"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="26"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1755,765 +1751,765 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:27" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="35" t="s">
+    <row r="19" spans="2:27" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="36" t="s">
+      <c r="C19" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="36" t="s">
+      <c r="D19" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E19" s="36" t="s">
+      <c r="E19" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="36" t="s">
+      <c r="F19" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="G19" s="37" t="s">
+      <c r="G19" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
-      <c r="L19" s="38"/>
-      <c r="M19" s="38"/>
-      <c r="N19" s="38"/>
-      <c r="O19" s="38"/>
-      <c r="P19" s="38"/>
-      <c r="Q19" s="38"/>
-      <c r="R19" s="38"/>
-      <c r="S19" s="38"/>
-      <c r="T19" s="38"/>
-      <c r="U19" s="38"/>
-      <c r="V19" s="38"/>
-      <c r="W19" s="38"/>
-      <c r="X19" s="38"/>
-      <c r="Y19" s="38"/>
-      <c r="Z19" s="38"/>
-      <c r="AA19" s="38"/>
-    </row>
-    <row r="20" spans="2:27" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="35" t="s">
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="27"/>
+      <c r="O19" s="27"/>
+      <c r="P19" s="27"/>
+      <c r="Q19" s="27"/>
+      <c r="R19" s="27"/>
+      <c r="S19" s="27"/>
+      <c r="T19" s="27"/>
+      <c r="U19" s="27"/>
+      <c r="V19" s="27"/>
+      <c r="W19" s="27"/>
+      <c r="X19" s="27"/>
+      <c r="Y19" s="27"/>
+      <c r="Z19" s="27"/>
+      <c r="AA19" s="27"/>
+    </row>
+    <row r="20" spans="2:27" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="36">
+      <c r="C20" s="25">
         <v>6</v>
       </c>
-      <c r="D20" s="36">
+      <c r="D20" s="25">
         <v>6</v>
       </c>
-      <c r="E20" s="36">
-        <v>0</v>
-      </c>
-      <c r="F20" s="36">
-        <v>0</v>
-      </c>
-      <c r="G20" s="37">
-        <v>0</v>
-      </c>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="38"/>
-      <c r="N20" s="38"/>
-      <c r="O20" s="38"/>
-      <c r="P20" s="38"/>
-      <c r="Q20" s="38"/>
-      <c r="R20" s="38"/>
-      <c r="S20" s="38"/>
-      <c r="T20" s="38"/>
-      <c r="U20" s="38"/>
-      <c r="V20" s="38"/>
-      <c r="W20" s="38"/>
-      <c r="X20" s="38"/>
-      <c r="Y20" s="38"/>
-      <c r="Z20" s="38"/>
-      <c r="AA20" s="38"/>
-    </row>
-    <row r="21" spans="2:27" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="35" t="s">
+      <c r="E20" s="25">
+        <v>0</v>
+      </c>
+      <c r="F20" s="25">
+        <v>0</v>
+      </c>
+      <c r="G20" s="26">
+        <v>0</v>
+      </c>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="27"/>
+      <c r="Q20" s="27"/>
+      <c r="R20" s="27"/>
+      <c r="S20" s="27"/>
+      <c r="T20" s="27"/>
+      <c r="U20" s="27"/>
+      <c r="V20" s="27"/>
+      <c r="W20" s="27"/>
+      <c r="X20" s="27"/>
+      <c r="Y20" s="27"/>
+      <c r="Z20" s="27"/>
+      <c r="AA20" s="27"/>
+    </row>
+    <row r="21" spans="2:27" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="36">
+      <c r="C21" s="25">
         <v>12</v>
       </c>
-      <c r="D21" s="36">
+      <c r="D21" s="25">
         <v>4</v>
       </c>
-      <c r="E21" s="36">
-        <v>0</v>
-      </c>
-      <c r="F21" s="36">
-        <v>0</v>
-      </c>
-      <c r="G21" s="37">
-        <v>0</v>
-      </c>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38"/>
-      <c r="K21" s="38"/>
-      <c r="L21" s="38"/>
-      <c r="M21" s="38"/>
-      <c r="N21" s="38"/>
-      <c r="O21" s="38"/>
-      <c r="P21" s="38"/>
-      <c r="Q21" s="38"/>
-      <c r="R21" s="38"/>
-      <c r="S21" s="38"/>
-      <c r="T21" s="38"/>
-      <c r="U21" s="38"/>
-      <c r="V21" s="38"/>
-      <c r="W21" s="38"/>
-      <c r="X21" s="38"/>
-      <c r="Y21" s="38"/>
-      <c r="Z21" s="38"/>
-      <c r="AA21" s="38"/>
-    </row>
-    <row r="22" spans="2:27" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="35" t="s">
+      <c r="E21" s="25">
+        <v>0</v>
+      </c>
+      <c r="F21" s="25">
+        <v>0</v>
+      </c>
+      <c r="G21" s="26">
+        <v>0</v>
+      </c>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="27"/>
+      <c r="Q21" s="27"/>
+      <c r="R21" s="27"/>
+      <c r="S21" s="27"/>
+      <c r="T21" s="27"/>
+      <c r="U21" s="27"/>
+      <c r="V21" s="27"/>
+      <c r="W21" s="27"/>
+      <c r="X21" s="27"/>
+      <c r="Y21" s="27"/>
+      <c r="Z21" s="27"/>
+      <c r="AA21" s="27"/>
+    </row>
+    <row r="22" spans="2:27" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="36">
+      <c r="C22" s="25">
         <v>16</v>
       </c>
-      <c r="D22" s="36">
+      <c r="D22" s="25">
         <v>2</v>
       </c>
-      <c r="E22" s="36">
-        <v>0</v>
-      </c>
-      <c r="F22" s="36">
-        <v>0</v>
-      </c>
-      <c r="G22" s="37">
-        <v>0</v>
-      </c>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="38"/>
-      <c r="M22" s="38"/>
-      <c r="N22" s="38"/>
-      <c r="O22" s="38"/>
-      <c r="P22" s="38"/>
-      <c r="Q22" s="38"/>
-      <c r="R22" s="38"/>
-      <c r="S22" s="38"/>
-      <c r="T22" s="38"/>
-      <c r="U22" s="38"/>
-      <c r="V22" s="38"/>
-      <c r="W22" s="38"/>
-      <c r="X22" s="38"/>
-      <c r="Y22" s="38"/>
-      <c r="Z22" s="38"/>
-      <c r="AA22" s="38"/>
-    </row>
-    <row r="23" spans="2:27" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="35" t="s">
+      <c r="E22" s="25">
+        <v>0</v>
+      </c>
+      <c r="F22" s="25">
+        <v>0</v>
+      </c>
+      <c r="G22" s="26">
+        <v>0</v>
+      </c>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="27"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="27"/>
+      <c r="Q22" s="27"/>
+      <c r="R22" s="27"/>
+      <c r="S22" s="27"/>
+      <c r="T22" s="27"/>
+      <c r="U22" s="27"/>
+      <c r="V22" s="27"/>
+      <c r="W22" s="27"/>
+      <c r="X22" s="27"/>
+      <c r="Y22" s="27"/>
+      <c r="Z22" s="27"/>
+      <c r="AA22" s="27"/>
+    </row>
+    <row r="23" spans="2:27" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="36">
+      <c r="C23" s="25">
         <v>18</v>
       </c>
-      <c r="D23" s="36">
+      <c r="D23" s="25">
         <v>4</v>
       </c>
-      <c r="E23" s="36">
-        <v>0</v>
-      </c>
-      <c r="F23" s="36">
-        <v>0</v>
-      </c>
-      <c r="G23" s="37">
-        <v>0</v>
-      </c>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="38"/>
-      <c r="K23" s="38"/>
-      <c r="L23" s="38"/>
-      <c r="M23" s="38"/>
-      <c r="N23" s="38"/>
-      <c r="O23" s="38"/>
-      <c r="P23" s="38"/>
-      <c r="Q23" s="38"/>
-      <c r="R23" s="38"/>
-      <c r="S23" s="38"/>
-      <c r="T23" s="38"/>
-      <c r="U23" s="38"/>
-      <c r="V23" s="38"/>
-      <c r="W23" s="38"/>
-      <c r="X23" s="38"/>
-      <c r="Y23" s="38"/>
-      <c r="Z23" s="38"/>
-      <c r="AA23" s="38"/>
-    </row>
-    <row r="24" spans="2:27" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="35" t="s">
+      <c r="E23" s="25">
+        <v>0</v>
+      </c>
+      <c r="F23" s="25">
+        <v>0</v>
+      </c>
+      <c r="G23" s="26">
+        <v>0</v>
+      </c>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="27"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="27"/>
+      <c r="Q23" s="27"/>
+      <c r="R23" s="27"/>
+      <c r="S23" s="27"/>
+      <c r="T23" s="27"/>
+      <c r="U23" s="27"/>
+      <c r="V23" s="27"/>
+      <c r="W23" s="27"/>
+      <c r="X23" s="27"/>
+      <c r="Y23" s="27"/>
+      <c r="Z23" s="27"/>
+      <c r="AA23" s="27"/>
+    </row>
+    <row r="24" spans="2:27" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="36">
+      <c r="C24" s="25">
         <v>2</v>
       </c>
-      <c r="D24" s="36">
+      <c r="D24" s="25">
         <v>4</v>
       </c>
-      <c r="E24" s="36">
+      <c r="E24" s="25">
         <v>3</v>
       </c>
-      <c r="F24" s="36">
-        <v>0</v>
-      </c>
-      <c r="G24" s="37">
+      <c r="F24" s="25">
+        <v>0</v>
+      </c>
+      <c r="G24" s="26">
         <v>0.05</v>
       </c>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="38"/>
-      <c r="L24" s="38"/>
-      <c r="M24" s="38"/>
-      <c r="N24" s="38"/>
-      <c r="O24" s="38"/>
-      <c r="P24" s="38"/>
-      <c r="Q24" s="38"/>
-      <c r="R24" s="38"/>
-      <c r="S24" s="38"/>
-      <c r="T24" s="38"/>
-      <c r="U24" s="38"/>
-      <c r="V24" s="38"/>
-      <c r="W24" s="38"/>
-      <c r="X24" s="38"/>
-      <c r="Y24" s="38"/>
-      <c r="Z24" s="38"/>
-      <c r="AA24" s="38"/>
-    </row>
-    <row r="25" spans="2:27" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="35" t="s">
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="27"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="27"/>
+      <c r="Q24" s="27"/>
+      <c r="R24" s="27"/>
+      <c r="S24" s="27"/>
+      <c r="T24" s="27"/>
+      <c r="U24" s="27"/>
+      <c r="V24" s="27"/>
+      <c r="W24" s="27"/>
+      <c r="X24" s="27"/>
+      <c r="Y24" s="27"/>
+      <c r="Z24" s="27"/>
+      <c r="AA24" s="27"/>
+    </row>
+    <row r="25" spans="2:27" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="36">
+      <c r="C25" s="25">
         <v>4</v>
       </c>
-      <c r="D25" s="36">
+      <c r="D25" s="25">
         <v>1</v>
       </c>
-      <c r="E25" s="36">
+      <c r="E25" s="25">
         <v>4</v>
       </c>
-      <c r="F25" s="36">
-        <v>0</v>
-      </c>
-      <c r="G25" s="37">
-        <v>0</v>
-      </c>
-      <c r="H25" s="38"/>
-      <c r="I25" s="38"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="38"/>
-      <c r="L25" s="38"/>
-      <c r="M25" s="38"/>
-      <c r="N25" s="38"/>
-      <c r="O25" s="38"/>
-      <c r="P25" s="38"/>
-      <c r="Q25" s="38"/>
-      <c r="R25" s="38"/>
-      <c r="S25" s="38"/>
-      <c r="T25" s="38"/>
-      <c r="U25" s="38"/>
-      <c r="V25" s="38"/>
-      <c r="W25" s="38"/>
-      <c r="X25" s="38"/>
-      <c r="Y25" s="38"/>
-      <c r="Z25" s="38"/>
-      <c r="AA25" s="38"/>
-    </row>
-    <row r="26" spans="2:27" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="35" t="s">
+      <c r="F25" s="25">
+        <v>0</v>
+      </c>
+      <c r="G25" s="26">
+        <v>0</v>
+      </c>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="27"/>
+      <c r="N25" s="27"/>
+      <c r="O25" s="27"/>
+      <c r="P25" s="27"/>
+      <c r="Q25" s="27"/>
+      <c r="R25" s="27"/>
+      <c r="S25" s="27"/>
+      <c r="T25" s="27"/>
+      <c r="U25" s="27"/>
+      <c r="V25" s="27"/>
+      <c r="W25" s="27"/>
+      <c r="X25" s="27"/>
+      <c r="Y25" s="27"/>
+      <c r="Z25" s="27"/>
+      <c r="AA25" s="27"/>
+    </row>
+    <row r="26" spans="2:27" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="36">
+      <c r="C26" s="25">
         <v>22</v>
       </c>
-      <c r="D26" s="36">
+      <c r="D26" s="25">
         <v>4</v>
       </c>
-      <c r="E26" s="36">
-        <v>0</v>
-      </c>
-      <c r="F26" s="36">
-        <v>0</v>
-      </c>
-      <c r="G26" s="37">
-        <v>0</v>
-      </c>
-      <c r="H26" s="38"/>
-      <c r="I26" s="38"/>
-      <c r="J26" s="38"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="38"/>
-      <c r="M26" s="38"/>
-      <c r="N26" s="38"/>
-      <c r="O26" s="38"/>
-      <c r="P26" s="38"/>
-      <c r="Q26" s="38"/>
-      <c r="R26" s="38"/>
-      <c r="S26" s="38"/>
-      <c r="T26" s="38"/>
-      <c r="U26" s="38"/>
-      <c r="V26" s="38"/>
-      <c r="W26" s="38"/>
-      <c r="X26" s="38"/>
-      <c r="Y26" s="38"/>
-      <c r="Z26" s="38"/>
-      <c r="AA26" s="38"/>
-    </row>
-    <row r="27" spans="2:27" s="44" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="40" t="s">
+      <c r="E26" s="25">
+        <v>0</v>
+      </c>
+      <c r="F26" s="25">
+        <v>0</v>
+      </c>
+      <c r="G26" s="26">
+        <v>0</v>
+      </c>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="27"/>
+      <c r="N26" s="27"/>
+      <c r="O26" s="27"/>
+      <c r="P26" s="27"/>
+      <c r="Q26" s="27"/>
+      <c r="R26" s="27"/>
+      <c r="S26" s="27"/>
+      <c r="T26" s="27"/>
+      <c r="U26" s="27"/>
+      <c r="V26" s="27"/>
+      <c r="W26" s="27"/>
+      <c r="X26" s="27"/>
+      <c r="Y26" s="27"/>
+      <c r="Z26" s="27"/>
+      <c r="AA26" s="27"/>
+    </row>
+    <row r="27" spans="2:27" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="41" t="s">
+      <c r="C27" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="41" t="s">
+      <c r="D27" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="41" t="s">
+      <c r="E27" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="41" t="s">
+      <c r="F27" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="G27" s="42" t="s">
+      <c r="G27" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="43"/>
-      <c r="L27" s="43"/>
-      <c r="M27" s="43"/>
-      <c r="N27" s="43"/>
-      <c r="O27" s="43"/>
-      <c r="P27" s="43"/>
-      <c r="Q27" s="43"/>
-      <c r="R27" s="43"/>
-      <c r="S27" s="43"/>
-      <c r="T27" s="43"/>
-      <c r="U27" s="43"/>
-      <c r="V27" s="43"/>
-      <c r="W27" s="43"/>
-      <c r="X27" s="43"/>
-      <c r="Y27" s="43"/>
-      <c r="Z27" s="43"/>
-      <c r="AA27" s="43"/>
-    </row>
-    <row r="28" spans="2:27" s="44" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="40" t="s">
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="32"/>
+      <c r="P27" s="32"/>
+      <c r="Q27" s="32"/>
+      <c r="R27" s="32"/>
+      <c r="S27" s="32"/>
+      <c r="T27" s="32"/>
+      <c r="U27" s="32"/>
+      <c r="V27" s="32"/>
+      <c r="W27" s="32"/>
+      <c r="X27" s="32"/>
+      <c r="Y27" s="32"/>
+      <c r="Z27" s="32"/>
+      <c r="AA27" s="32"/>
+    </row>
+    <row r="28" spans="2:27" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="41">
+      <c r="C28" s="30">
         <v>4</v>
       </c>
-      <c r="D28" s="41">
+      <c r="D28" s="30">
         <v>2</v>
       </c>
-      <c r="E28" s="41">
-        <v>0</v>
-      </c>
-      <c r="F28" s="41">
-        <v>0</v>
-      </c>
-      <c r="G28" s="42">
-        <v>0</v>
-      </c>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
-      <c r="K28" s="43"/>
-      <c r="L28" s="43"/>
-      <c r="M28" s="43"/>
-      <c r="N28" s="43"/>
-      <c r="O28" s="43"/>
-      <c r="P28" s="43"/>
-      <c r="Q28" s="43"/>
-      <c r="R28" s="43"/>
-      <c r="S28" s="43"/>
-      <c r="T28" s="43"/>
-      <c r="U28" s="43"/>
-      <c r="V28" s="43"/>
-      <c r="W28" s="43"/>
-      <c r="X28" s="43"/>
-      <c r="Y28" s="43"/>
-      <c r="Z28" s="43"/>
-      <c r="AA28" s="43"/>
-    </row>
-    <row r="29" spans="2:27" s="44" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="40" t="s">
+      <c r="E28" s="30">
+        <v>0</v>
+      </c>
+      <c r="F28" s="30">
+        <v>0</v>
+      </c>
+      <c r="G28" s="31">
+        <v>0</v>
+      </c>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="32"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="32"/>
+      <c r="O28" s="32"/>
+      <c r="P28" s="32"/>
+      <c r="Q28" s="32"/>
+      <c r="R28" s="32"/>
+      <c r="S28" s="32"/>
+      <c r="T28" s="32"/>
+      <c r="U28" s="32"/>
+      <c r="V28" s="32"/>
+      <c r="W28" s="32"/>
+      <c r="X28" s="32"/>
+      <c r="Y28" s="32"/>
+      <c r="Z28" s="32"/>
+      <c r="AA28" s="32"/>
+    </row>
+    <row r="29" spans="2:27" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="41">
+      <c r="C29" s="30">
         <v>6</v>
       </c>
-      <c r="D29" s="41">
+      <c r="D29" s="30">
         <v>1</v>
       </c>
-      <c r="E29" s="41">
-        <v>0</v>
-      </c>
-      <c r="F29" s="41">
-        <v>0</v>
-      </c>
-      <c r="G29" s="42">
-        <v>0</v>
-      </c>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="43"/>
-      <c r="L29" s="43"/>
-      <c r="M29" s="43"/>
-      <c r="N29" s="43"/>
-      <c r="O29" s="43"/>
-      <c r="P29" s="43"/>
-      <c r="Q29" s="43"/>
-      <c r="R29" s="43"/>
-      <c r="S29" s="43"/>
-      <c r="T29" s="43"/>
-      <c r="U29" s="43"/>
-      <c r="V29" s="43"/>
-      <c r="W29" s="43"/>
-      <c r="X29" s="43"/>
-      <c r="Y29" s="43"/>
-      <c r="Z29" s="43"/>
-      <c r="AA29" s="43"/>
-    </row>
-    <row r="30" spans="2:27" s="44" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="40" t="s">
+      <c r="E29" s="30">
+        <v>0</v>
+      </c>
+      <c r="F29" s="30">
+        <v>0</v>
+      </c>
+      <c r="G29" s="31">
+        <v>0</v>
+      </c>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="32"/>
+      <c r="L29" s="32"/>
+      <c r="M29" s="32"/>
+      <c r="N29" s="32"/>
+      <c r="O29" s="32"/>
+      <c r="P29" s="32"/>
+      <c r="Q29" s="32"/>
+      <c r="R29" s="32"/>
+      <c r="S29" s="32"/>
+      <c r="T29" s="32"/>
+      <c r="U29" s="32"/>
+      <c r="V29" s="32"/>
+      <c r="W29" s="32"/>
+      <c r="X29" s="32"/>
+      <c r="Y29" s="32"/>
+      <c r="Z29" s="32"/>
+      <c r="AA29" s="32"/>
+    </row>
+    <row r="30" spans="2:27" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="41">
+      <c r="C30" s="30">
         <v>8</v>
       </c>
-      <c r="D30" s="41">
+      <c r="D30" s="30">
         <v>1</v>
       </c>
-      <c r="E30" s="41">
-        <v>0</v>
-      </c>
-      <c r="F30" s="41">
-        <v>0</v>
-      </c>
-      <c r="G30" s="42">
-        <v>0</v>
-      </c>
-      <c r="H30" s="43"/>
-      <c r="I30" s="43"/>
-      <c r="J30" s="43"/>
-      <c r="K30" s="43"/>
-      <c r="L30" s="43"/>
-      <c r="M30" s="43"/>
-      <c r="N30" s="43"/>
-      <c r="O30" s="43"/>
-      <c r="P30" s="43"/>
-      <c r="Q30" s="43"/>
-      <c r="R30" s="43"/>
-      <c r="S30" s="43"/>
-      <c r="T30" s="43"/>
-      <c r="U30" s="43"/>
-      <c r="V30" s="43"/>
-      <c r="W30" s="43"/>
-      <c r="X30" s="43"/>
-      <c r="Y30" s="43"/>
-      <c r="Z30" s="43"/>
-      <c r="AA30" s="43"/>
-    </row>
-    <row r="31" spans="2:27" s="44" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="40" t="s">
+      <c r="E30" s="30">
+        <v>0</v>
+      </c>
+      <c r="F30" s="30">
+        <v>0</v>
+      </c>
+      <c r="G30" s="31">
+        <v>0</v>
+      </c>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="32"/>
+      <c r="O30" s="32"/>
+      <c r="P30" s="32"/>
+      <c r="Q30" s="32"/>
+      <c r="R30" s="32"/>
+      <c r="S30" s="32"/>
+      <c r="T30" s="32"/>
+      <c r="U30" s="32"/>
+      <c r="V30" s="32"/>
+      <c r="W30" s="32"/>
+      <c r="X30" s="32"/>
+      <c r="Y30" s="32"/>
+      <c r="Z30" s="32"/>
+      <c r="AA30" s="32"/>
+    </row>
+    <row r="31" spans="2:27" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="41">
+      <c r="C31" s="30">
         <v>12</v>
       </c>
-      <c r="D31" s="41">
+      <c r="D31" s="30">
         <v>2</v>
       </c>
-      <c r="E31" s="41">
-        <v>0</v>
-      </c>
-      <c r="F31" s="41">
-        <v>0</v>
-      </c>
-      <c r="G31" s="42">
-        <v>0</v>
-      </c>
-      <c r="H31" s="43"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="43"/>
-      <c r="K31" s="43"/>
-      <c r="L31" s="43"/>
-      <c r="M31" s="43"/>
-      <c r="N31" s="43"/>
-      <c r="O31" s="43"/>
-      <c r="P31" s="43"/>
-      <c r="Q31" s="43"/>
-      <c r="R31" s="43"/>
-      <c r="S31" s="43"/>
-      <c r="T31" s="43"/>
-      <c r="U31" s="43"/>
-      <c r="V31" s="43"/>
-      <c r="W31" s="43"/>
-      <c r="X31" s="43"/>
-      <c r="Y31" s="43"/>
-      <c r="Z31" s="43"/>
-      <c r="AA31" s="43"/>
-    </row>
-    <row r="32" spans="2:27" s="44" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="40" t="s">
+      <c r="E31" s="30">
+        <v>0</v>
+      </c>
+      <c r="F31" s="30">
+        <v>0</v>
+      </c>
+      <c r="G31" s="31">
+        <v>0</v>
+      </c>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="32"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="32"/>
+      <c r="O31" s="32"/>
+      <c r="P31" s="32"/>
+      <c r="Q31" s="32"/>
+      <c r="R31" s="32"/>
+      <c r="S31" s="32"/>
+      <c r="T31" s="32"/>
+      <c r="U31" s="32"/>
+      <c r="V31" s="32"/>
+      <c r="W31" s="32"/>
+      <c r="X31" s="32"/>
+      <c r="Y31" s="32"/>
+      <c r="Z31" s="32"/>
+      <c r="AA31" s="32"/>
+    </row>
+    <row r="32" spans="2:27" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="41">
+      <c r="C32" s="30">
         <v>15</v>
       </c>
-      <c r="D32" s="41">
+      <c r="D32" s="30">
         <v>4</v>
       </c>
-      <c r="E32" s="41">
-        <v>0</v>
-      </c>
-      <c r="F32" s="41">
-        <v>0</v>
-      </c>
-      <c r="G32" s="42">
-        <v>0</v>
-      </c>
-      <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
-      <c r="J32" s="43"/>
-      <c r="K32" s="43"/>
-      <c r="L32" s="43"/>
-      <c r="M32" s="43"/>
-      <c r="N32" s="43"/>
-      <c r="O32" s="43"/>
-      <c r="P32" s="43"/>
-      <c r="Q32" s="43"/>
-      <c r="R32" s="43"/>
-      <c r="S32" s="43"/>
-      <c r="T32" s="43"/>
-      <c r="U32" s="43"/>
-      <c r="V32" s="43"/>
-      <c r="W32" s="43"/>
-      <c r="X32" s="43"/>
-      <c r="Y32" s="43"/>
-      <c r="Z32" s="43"/>
-      <c r="AA32" s="43"/>
-    </row>
-    <row r="33" spans="2:27" s="44" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="40" t="s">
+      <c r="E32" s="30">
+        <v>0</v>
+      </c>
+      <c r="F32" s="30">
+        <v>0</v>
+      </c>
+      <c r="G32" s="31">
+        <v>0</v>
+      </c>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="32"/>
+      <c r="L32" s="32"/>
+      <c r="M32" s="32"/>
+      <c r="N32" s="32"/>
+      <c r="O32" s="32"/>
+      <c r="P32" s="32"/>
+      <c r="Q32" s="32"/>
+      <c r="R32" s="32"/>
+      <c r="S32" s="32"/>
+      <c r="T32" s="32"/>
+      <c r="U32" s="32"/>
+      <c r="V32" s="32"/>
+      <c r="W32" s="32"/>
+      <c r="X32" s="32"/>
+      <c r="Y32" s="32"/>
+      <c r="Z32" s="32"/>
+      <c r="AA32" s="32"/>
+    </row>
+    <row r="33" spans="2:27" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="41">
+      <c r="C33" s="30">
         <v>19</v>
       </c>
-      <c r="D33" s="41">
+      <c r="D33" s="30">
         <v>1</v>
       </c>
-      <c r="E33" s="41">
-        <v>0</v>
-      </c>
-      <c r="F33" s="41">
-        <v>0</v>
-      </c>
-      <c r="G33" s="42">
-        <v>0</v>
-      </c>
-      <c r="H33" s="43"/>
-      <c r="I33" s="43"/>
-      <c r="J33" s="43"/>
-      <c r="K33" s="43"/>
-      <c r="L33" s="43"/>
-      <c r="M33" s="43"/>
-      <c r="N33" s="43"/>
-      <c r="O33" s="43"/>
-      <c r="P33" s="43"/>
-      <c r="Q33" s="43"/>
-      <c r="R33" s="43"/>
-      <c r="S33" s="43"/>
-      <c r="T33" s="43"/>
-      <c r="U33" s="43"/>
-      <c r="V33" s="43"/>
-      <c r="W33" s="43"/>
-      <c r="X33" s="43"/>
-      <c r="Y33" s="43"/>
-      <c r="Z33" s="43"/>
-      <c r="AA33" s="43"/>
-    </row>
-    <row r="34" spans="2:27" s="44" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="40" t="s">
+      <c r="E33" s="30">
+        <v>0</v>
+      </c>
+      <c r="F33" s="30">
+        <v>0</v>
+      </c>
+      <c r="G33" s="31">
+        <v>0</v>
+      </c>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="32"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="32"/>
+      <c r="N33" s="32"/>
+      <c r="O33" s="32"/>
+      <c r="P33" s="32"/>
+      <c r="Q33" s="32"/>
+      <c r="R33" s="32"/>
+      <c r="S33" s="32"/>
+      <c r="T33" s="32"/>
+      <c r="U33" s="32"/>
+      <c r="V33" s="32"/>
+      <c r="W33" s="32"/>
+      <c r="X33" s="32"/>
+      <c r="Y33" s="32"/>
+      <c r="Z33" s="32"/>
+      <c r="AA33" s="32"/>
+    </row>
+    <row r="34" spans="2:27" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="41">
+      <c r="C34" s="30">
         <v>20</v>
       </c>
-      <c r="D34" s="41">
+      <c r="D34" s="30">
         <v>2</v>
       </c>
-      <c r="E34" s="41">
-        <v>0</v>
-      </c>
-      <c r="F34" s="41">
-        <v>0</v>
-      </c>
-      <c r="G34" s="42">
-        <v>0</v>
-      </c>
-      <c r="H34" s="43"/>
-      <c r="I34" s="43"/>
-      <c r="J34" s="43"/>
-      <c r="K34" s="43"/>
-      <c r="L34" s="43"/>
-      <c r="M34" s="43"/>
-      <c r="N34" s="43"/>
-      <c r="O34" s="43"/>
-      <c r="P34" s="43"/>
-      <c r="Q34" s="43"/>
-      <c r="R34" s="43"/>
-      <c r="S34" s="43"/>
-      <c r="T34" s="43"/>
-      <c r="U34" s="43"/>
-      <c r="V34" s="43"/>
-      <c r="W34" s="43"/>
-      <c r="X34" s="43"/>
-      <c r="Y34" s="43"/>
-      <c r="Z34" s="43"/>
-      <c r="AA34" s="43"/>
-    </row>
-    <row r="35" spans="2:27" s="44" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="40" t="s">
+      <c r="E34" s="30">
+        <v>0</v>
+      </c>
+      <c r="F34" s="30">
+        <v>0</v>
+      </c>
+      <c r="G34" s="31">
+        <v>0</v>
+      </c>
+      <c r="H34" s="32"/>
+      <c r="I34" s="32"/>
+      <c r="J34" s="32"/>
+      <c r="K34" s="32"/>
+      <c r="L34" s="32"/>
+      <c r="M34" s="32"/>
+      <c r="N34" s="32"/>
+      <c r="O34" s="32"/>
+      <c r="P34" s="32"/>
+      <c r="Q34" s="32"/>
+      <c r="R34" s="32"/>
+      <c r="S34" s="32"/>
+      <c r="T34" s="32"/>
+      <c r="U34" s="32"/>
+      <c r="V34" s="32"/>
+      <c r="W34" s="32"/>
+      <c r="X34" s="32"/>
+      <c r="Y34" s="32"/>
+      <c r="Z34" s="32"/>
+      <c r="AA34" s="32"/>
+    </row>
+    <row r="35" spans="2:27" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="41">
+      <c r="C35" s="30">
         <v>2</v>
       </c>
-      <c r="D35" s="41">
+      <c r="D35" s="30">
         <v>4</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="30">
         <v>2</v>
       </c>
-      <c r="F35" s="41">
-        <v>0</v>
-      </c>
-      <c r="G35" s="42">
+      <c r="F35" s="30">
+        <v>0</v>
+      </c>
+      <c r="G35" s="31">
         <v>0.05</v>
       </c>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="43"/>
-      <c r="K35" s="43"/>
-      <c r="L35" s="43"/>
-      <c r="M35" s="43"/>
-      <c r="N35" s="43"/>
-      <c r="O35" s="43"/>
-      <c r="P35" s="43"/>
-      <c r="Q35" s="43"/>
-      <c r="R35" s="43"/>
-      <c r="S35" s="43"/>
-      <c r="T35" s="43"/>
-      <c r="U35" s="43"/>
-      <c r="V35" s="43"/>
-      <c r="W35" s="43"/>
-      <c r="X35" s="43"/>
-      <c r="Y35" s="43"/>
-      <c r="Z35" s="43"/>
-      <c r="AA35" s="43"/>
-    </row>
-    <row r="36" spans="2:27" s="44" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="40" t="s">
+      <c r="H35" s="32"/>
+      <c r="I35" s="32"/>
+      <c r="J35" s="32"/>
+      <c r="K35" s="32"/>
+      <c r="L35" s="32"/>
+      <c r="M35" s="32"/>
+      <c r="N35" s="32"/>
+      <c r="O35" s="32"/>
+      <c r="P35" s="32"/>
+      <c r="Q35" s="32"/>
+      <c r="R35" s="32"/>
+      <c r="S35" s="32"/>
+      <c r="T35" s="32"/>
+      <c r="U35" s="32"/>
+      <c r="V35" s="32"/>
+      <c r="W35" s="32"/>
+      <c r="X35" s="32"/>
+      <c r="Y35" s="32"/>
+      <c r="Z35" s="32"/>
+      <c r="AA35" s="32"/>
+    </row>
+    <row r="36" spans="2:27" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="41">
+      <c r="C36" s="30">
         <v>3</v>
       </c>
-      <c r="D36" s="41">
+      <c r="D36" s="30">
         <v>1</v>
       </c>
-      <c r="E36" s="41">
-        <v>0</v>
-      </c>
-      <c r="F36" s="41">
-        <v>0</v>
-      </c>
-      <c r="G36" s="42">
-        <v>0</v>
-      </c>
-      <c r="H36" s="43"/>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
-      <c r="K36" s="43"/>
-      <c r="L36" s="43"/>
-      <c r="M36" s="43"/>
-      <c r="N36" s="43"/>
-      <c r="O36" s="43"/>
-      <c r="P36" s="43"/>
-      <c r="Q36" s="43"/>
-      <c r="R36" s="43"/>
-      <c r="S36" s="43"/>
-      <c r="T36" s="43"/>
-      <c r="U36" s="43"/>
-      <c r="V36" s="43"/>
-      <c r="W36" s="43"/>
-      <c r="X36" s="43"/>
-      <c r="Y36" s="43"/>
-      <c r="Z36" s="43"/>
-      <c r="AA36" s="43"/>
-    </row>
-    <row r="37" spans="2:27" s="44" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="40" t="s">
+      <c r="E36" s="30">
+        <v>0</v>
+      </c>
+      <c r="F36" s="30">
+        <v>0</v>
+      </c>
+      <c r="G36" s="31">
+        <v>0</v>
+      </c>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="32"/>
+      <c r="L36" s="32"/>
+      <c r="M36" s="32"/>
+      <c r="N36" s="32"/>
+      <c r="O36" s="32"/>
+      <c r="P36" s="32"/>
+      <c r="Q36" s="32"/>
+      <c r="R36" s="32"/>
+      <c r="S36" s="32"/>
+      <c r="T36" s="32"/>
+      <c r="U36" s="32"/>
+      <c r="V36" s="32"/>
+      <c r="W36" s="32"/>
+      <c r="X36" s="32"/>
+      <c r="Y36" s="32"/>
+      <c r="Z36" s="32"/>
+      <c r="AA36" s="32"/>
+    </row>
+    <row r="37" spans="2:27" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="41">
+      <c r="C37" s="30">
         <v>22</v>
       </c>
-      <c r="D37" s="41">
+      <c r="D37" s="30">
         <v>4</v>
       </c>
-      <c r="E37" s="41">
-        <v>0</v>
-      </c>
-      <c r="F37" s="41">
-        <v>0</v>
-      </c>
-      <c r="G37" s="42">
-        <v>0</v>
-      </c>
-      <c r="H37" s="43"/>
-      <c r="I37" s="43"/>
-      <c r="J37" s="43"/>
-      <c r="K37" s="43"/>
-      <c r="L37" s="43"/>
-      <c r="M37" s="43"/>
-      <c r="N37" s="43"/>
-      <c r="O37" s="43"/>
-      <c r="P37" s="43"/>
-      <c r="Q37" s="43"/>
-      <c r="R37" s="43"/>
-      <c r="S37" s="43"/>
-      <c r="T37" s="43"/>
-      <c r="U37" s="43"/>
-      <c r="V37" s="43"/>
-      <c r="W37" s="43"/>
-      <c r="X37" s="43"/>
-      <c r="Y37" s="43"/>
-      <c r="Z37" s="43"/>
-      <c r="AA37" s="43"/>
+      <c r="E37" s="30">
+        <v>0</v>
+      </c>
+      <c r="F37" s="30">
+        <v>0</v>
+      </c>
+      <c r="G37" s="31">
+        <v>0</v>
+      </c>
+      <c r="H37" s="32"/>
+      <c r="I37" s="32"/>
+      <c r="J37" s="32"/>
+      <c r="K37" s="32"/>
+      <c r="L37" s="32"/>
+      <c r="M37" s="32"/>
+      <c r="N37" s="32"/>
+      <c r="O37" s="32"/>
+      <c r="P37" s="32"/>
+      <c r="Q37" s="32"/>
+      <c r="R37" s="32"/>
+      <c r="S37" s="32"/>
+      <c r="T37" s="32"/>
+      <c r="U37" s="32"/>
+      <c r="V37" s="32"/>
+      <c r="W37" s="32"/>
+      <c r="X37" s="32"/>
+      <c r="Y37" s="32"/>
+      <c r="Z37" s="32"/>
+      <c r="AA37" s="32"/>
     </row>
     <row r="38" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="23" t="s">
@@ -2805,7 +2801,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="16">
+  <dataValidations count="16">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>

</xml_diff>